<commit_message>
Update Controle de Materiais Estoque.xlsx
</commit_message>
<xml_diff>
--- a/Controle de Materiais Estoque.xlsx
+++ b/Controle de Materiais Estoque.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petrobrasbr-my.sharepoint.com/personal/afonsoverardi_prestserv_petrobras_com_br/Documents/Documentos/GitHub/dashboard-estoque/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_07F94E695743580F62355476585DCE3A87479C73" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7FE7C30-096C-43E8-8A65-01F6C236182E}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_07F94E695743580F62355476585DCE3A87479C73" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{703B79CA-9F19-4E2B-86CD-FF3250166AEA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="114">
   <si>
     <t>NM</t>
   </si>
@@ -191,12 +191,6 @@
   </si>
   <si>
     <t>Etiqueta seg. padrão PE-2RGN-00104 polie</t>
-  </si>
-  <si>
-    <t>11.245.954</t>
-  </si>
-  <si>
-    <t>Extintor incên. 80-B:C</t>
   </si>
   <si>
     <t>11.331.124</t>
@@ -443,6 +437,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -730,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,13 +1354,13 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
@@ -1370,22 +1368,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
         <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
@@ -1399,16 +1397,16 @@
         <v>68</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>10000</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="E29" t="s">
         <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
@@ -1416,19 +1414,19 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30">
+        <v>13000</v>
+      </c>
+      <c r="D30" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30">
-        <v>10000</v>
-      </c>
-      <c r="D30" t="s">
-        <v>71</v>
-      </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
@@ -1445,10 +1443,10 @@
         <v>73</v>
       </c>
       <c r="C31">
-        <v>13000</v>
+        <v>14000</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
@@ -1468,16 +1466,16 @@
         <v>75</v>
       </c>
       <c r="C32">
-        <v>14000</v>
+        <v>2500</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G32" t="s">
         <v>12</v>
@@ -1491,13 +1489,13 @@
         <v>77</v>
       </c>
       <c r="C33">
-        <v>2500</v>
+        <v>4400</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F33" t="s">
         <v>20</v>
@@ -1514,13 +1512,13 @@
         <v>79</v>
       </c>
       <c r="C34">
-        <v>4400</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
         <v>20</v>
@@ -1546,7 +1544,7 @@
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="G35" t="s">
         <v>12</v>
@@ -1606,16 +1604,16 @@
         <v>87</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="F38" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>
@@ -1623,22 +1621,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C39">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="F39" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G39" t="s">
         <v>12</v>
@@ -1652,16 +1650,16 @@
         <v>93</v>
       </c>
       <c r="C40">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F40" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G40" t="s">
         <v>12</v>
@@ -1675,7 +1673,7 @@
         <v>95</v>
       </c>
       <c r="C41">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -1698,16 +1696,16 @@
         <v>97</v>
       </c>
       <c r="C42">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G42" t="s">
         <v>12</v>
@@ -1721,7 +1719,7 @@
         <v>99</v>
       </c>
       <c r="C43">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s">
         <v>9</v>
@@ -1744,16 +1742,16 @@
         <v>101</v>
       </c>
       <c r="C44">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>9</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F44" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="G44" t="s">
         <v>12</v>
@@ -1767,16 +1765,16 @@
         <v>103</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="E45" t="s">
         <v>14</v>
       </c>
       <c r="F45" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G45" t="s">
         <v>12</v>
@@ -1790,16 +1788,16 @@
         <v>105</v>
       </c>
       <c r="C46">
-        <v>5.8000000000000003E-2</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="G46" t="s">
         <v>12</v>
@@ -1813,7 +1811,7 @@
         <v>107</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
@@ -1822,7 +1820,7 @@
         <v>10</v>
       </c>
       <c r="F47" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G47" t="s">
         <v>12</v>
@@ -1836,7 +1834,7 @@
         <v>109</v>
       </c>
       <c r="C48">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D48" t="s">
         <v>9</v>
@@ -1859,13 +1857,13 @@
         <v>111</v>
       </c>
       <c r="C49">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F49" t="s">
         <v>11</v>
@@ -1894,29 +1892,6 @@
         <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>114</v>
-      </c>
-      <c r="B51" t="s">
-        <v>115</v>
-      </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>